<commit_message>
dept manager in admin
</commit_message>
<xml_diff>
--- a/assets/Consolidated list of API's.xlsx
+++ b/assets/Consolidated list of API's.xlsx
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1210,21 +1210,21 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" ht="129">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="129">
+      <c r="B15" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="51.75">
       <c r="B16" s="7" t="s">
@@ -1262,39 +1262,39 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="128.25">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="128.25">
+      <c r="B18" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="29.25">
-      <c r="B19" s="3" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" s="6" customFormat="1" ht="29.25">
+      <c r="B19" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" ht="30">
       <c r="B20" s="3" t="s">

</xml_diff>

<commit_message>
admin setting pages functionalities completed
</commit_message>
<xml_diff>
--- a/assets/Consolidated list of API's.xlsx
+++ b/assets/Consolidated list of API's.xlsx
@@ -624,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -656,9 +656,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -955,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1184,15 +1181,15 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:8" s="6" customFormat="1">
+      <c r="B13" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="57.75">
       <c r="B14" s="7" t="s">
@@ -1296,160 +1293,160 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="30">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:7" s="6" customFormat="1" ht="30">
+      <c r="B20" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" ht="57.75">
-      <c r="B21" s="3" t="s">
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" s="6" customFormat="1" ht="57.75">
+      <c r="B21" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="114.75">
-      <c r="B22" s="3" t="s">
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" s="6" customFormat="1" ht="114.75">
+      <c r="B22" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" ht="51.75">
-      <c r="B23" s="3" t="s">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" s="6" customFormat="1" ht="51.75">
+      <c r="B23" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" ht="51.75">
-      <c r="B24" s="3" t="s">
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="51.75">
+      <c r="B24" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" ht="26.25">
-      <c r="B25" s="3" t="s">
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="26.25">
+      <c r="B25" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" ht="45">
-      <c r="B26" s="5" t="s">
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="45">
+      <c r="B26" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="51.75">
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="51.75">
+      <c r="B27" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="2" customFormat="1">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="1:7" s="6" customFormat="1">
+      <c r="B28" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E28" s="15"/>
+      <c r="E28" s="16"/>
     </row>
     <row r="29" spans="1:7" s="6" customFormat="1" ht="60">
       <c r="B29" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1457,13 +1454,13 @@
       <c r="B30" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="15" t="s">
         <v>107</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>108</v>
       </c>
       <c r="F30" s="7" t="s">
@@ -1472,9 +1469,9 @@
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1">
       <c r="B31" s="5"/>
-      <c r="C31" s="14"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:7" s="6" customFormat="1" ht="102.75">
@@ -1590,10 +1587,10 @@
       <c r="B38" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="16" t="s">
         <v>116</v>
       </c>
       <c r="F38" s="6" t="s">
@@ -1605,13 +1602,13 @@
       <c r="B39" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="15" t="s">
         <v>117</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="16" t="s">
         <v>118</v>
       </c>
       <c r="F39" s="6" t="s">
@@ -1623,13 +1620,13 @@
       <c r="B40" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>121</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="14" t="s">
         <v>122</v>
       </c>
       <c r="F40" s="2" t="s">
@@ -1641,13 +1638,13 @@
       <c r="B41" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>124</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="14" t="s">
         <v>125</v>
       </c>
       <c r="F41" s="2" t="s">
@@ -1656,20 +1653,20 @@
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1">
-      <c r="E42" s="15"/>
+      <c r="E42" s="14"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" ht="30">
       <c r="B43" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="14" t="s">
         <v>128</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -1678,16 +1675,16 @@
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1">
-      <c r="E44" s="15"/>
+      <c r="E44" s="14"/>
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" ht="30">
       <c r="B45" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="14" t="s">
         <v>131</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -1695,19 +1692,19 @@
       </c>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1">
-      <c r="E46" s="15"/>
+      <c r="E46" s="14"/>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" ht="45">
       <c r="B47" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="13" t="s">
         <v>133</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="14" t="s">
         <v>134</v>
       </c>
       <c r="F47" s="2" t="s">
@@ -1778,10 +1775,10 @@
       <c r="D51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1795,7 +1792,7 @@
       <c r="D52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="17" t="s">
         <v>55</v>
       </c>
       <c r="F52" s="7" t="s">
@@ -1823,13 +1820,13 @@
       <c r="B54" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="15" t="s">
         <v>110</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="16" t="s">
         <v>111</v>
       </c>
       <c r="F54" s="6" t="s">
@@ -1840,13 +1837,13 @@
       <c r="B55" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="16" t="s">
         <v>113</v>
       </c>
       <c r="F55" s="6" t="s">

</xml_diff>